<commit_message>
Excel file und excel link update
</commit_message>
<xml_diff>
--- a/TicketBookingDataK.xlsx
+++ b/TicketBookingDataK.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\WptTicketBooking1github\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D474FFB-8189-418D-B45A-859E6E18B176}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BE13818C-E35E-4B15-96B0-725D12B74B71}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" activeTab="2" xr2:uid="{8B5DEFB1-BB2A-466C-9D9F-A1A8C6BAB584}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{8B5DEFB1-BB2A-466C-9D9F-A1A8C6BAB584}"/>
   </bookViews>
   <sheets>
     <sheet name="Users" sheetId="1" r:id="rId1"/>
@@ -449,7 +449,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:B5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
@@ -585,7 +585,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>

</xml_diff>